<commit_message>
cambios en fechas y seguridad de reg admin
</commit_message>
<xml_diff>
--- a/static/docs/Asistentes.xlsx
+++ b/static/docs/Asistentes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,32 +429,32 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Nombres</t>
+          <t>NOMBRES</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Apellidos</t>
+          <t>APELLIDOS</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Correo</t>
+          <t>CORREO</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Celular</t>
+          <t>CELULAR</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Empresa</t>
+          <t>EMPRESA</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Cargo</t>
+          <t>CARGO</t>
         </is>
       </c>
     </row>
@@ -474,7 +474,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>masutier@test.com</t>
+          <t>gabrielmasutier@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -484,47 +484,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Freelance</t>
+          <t>La Data Inquisición</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Liliana</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Guerrero</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>lilit@test.com</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>5553332121</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Ecopetrol</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Asistente Direccion</t>
+          <t>Analista</t>
         </is>
       </c>
     </row>

</xml_diff>